<commit_message>
Add substatus to work_type_statuses.xlsx
</commit_message>
<xml_diff>
--- a/src/definitions/worktypes/work_type_statuses.xlsx
+++ b/src/definitions/worktypes/work_type_statuses.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\GitHub\crisiscleanup-web\src\definitions\worktypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8140008_{CB52CBF3-E018-483D-9986-209FD1A13265}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B426345-59C1-4B4A-9AAE-7F2030FF9F2B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6615"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="work_type_statuses" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="100">
   <si>
     <t>|</t>
   </si>
@@ -28,42 +28,12 @@
     <t>||</t>
   </si>
   <si>
-    <t>||__name_t</t>
-  </si>
-  <si>
-    <t>||__description_t</t>
-  </si>
-  <si>
-    <t>||__claimed_class</t>
-  </si>
-  <si>
-    <t>||__unclaimed_class</t>
-  </si>
-  <si>
-    <t>||__completed_by_anybody</t>
-  </si>
-  <si>
-    <t>||__completed_by_ccu</t>
-  </si>
-  <si>
-    <t>||__completed_db</t>
-  </si>
-  <si>
-    <t>||__last_updated</t>
-  </si>
-  <si>
-    <t>||__depreciated_date</t>
-  </si>
-  <si>
     <t>open</t>
   </si>
   <si>
     <t>open_unassigned</t>
   </si>
   <si>
-    <t>status.open_unassigned</t>
-  </si>
-  <si>
     <t>open-unassigned-claimed</t>
   </si>
   <si>
@@ -76,9 +46,6 @@
     <t>open_assigned</t>
   </si>
   <si>
-    <t>status.open_assigned</t>
-  </si>
-  <si>
     <t>open-assigned-claimed</t>
   </si>
   <si>
@@ -88,9 +55,6 @@
     <t>open_partially_completed</t>
   </si>
   <si>
-    <t>status.open_partially_completed</t>
-  </si>
-  <si>
     <t>open-partially-completed-claimed</t>
   </si>
   <si>
@@ -100,9 +64,6 @@
     <t>open_needs_follow_up</t>
   </si>
   <si>
-    <t>status.open_needs_follow_up</t>
-  </si>
-  <si>
     <t>open-needs-follow-up-claimed</t>
   </si>
   <si>
@@ -112,9 +73,6 @@
     <t>open_unresponsive</t>
   </si>
   <si>
-    <t>status.open_unresponsive</t>
-  </si>
-  <si>
     <t>open-unresponsive-claimed</t>
   </si>
   <si>
@@ -127,9 +85,6 @@
     <t>closed_completed</t>
   </si>
   <si>
-    <t>status.closed_completed</t>
-  </si>
-  <si>
     <t>closed-completed-claimed</t>
   </si>
   <si>
@@ -139,9 +94,6 @@
     <t>closed_incomplete</t>
   </si>
   <si>
-    <t>status.closed_incomplete</t>
-  </si>
-  <si>
     <t>closed-incomplete-claimed</t>
   </si>
   <si>
@@ -151,9 +103,6 @@
     <t>closed_out_of_scope</t>
   </si>
   <si>
-    <t>status.closed_out_of_scope</t>
-  </si>
-  <si>
     <t>closed-out-of-scope-claimed</t>
   </si>
   <si>
@@ -163,9 +112,6 @@
     <t>closed_done_by_others</t>
   </si>
   <si>
-    <t>status.closed_done_by_others</t>
-  </si>
-  <si>
     <t>closed-done-by-others-claimed</t>
   </si>
   <si>
@@ -175,9 +121,6 @@
     <t>closed_no_help_wanted</t>
   </si>
   <si>
-    <t>status.closed_no_help_wanted</t>
-  </si>
-  <si>
     <t>closed-no-help-wanted-claimed</t>
   </si>
   <si>
@@ -187,9 +130,6 @@
     <t>closed_rejected</t>
   </si>
   <si>
-    <t>status.closed_rejected</t>
-  </si>
-  <si>
     <t>closed-rejected-claimed</t>
   </si>
   <si>
@@ -199,9 +139,6 @@
     <t>closed_duplicate</t>
   </si>
   <si>
-    <t>status.closed_duplicate</t>
-  </si>
-  <si>
     <t>closed-duplicate-claimed</t>
   </si>
   <si>
@@ -211,9 +148,6 @@
     <t>closed_marked_for_deletion</t>
   </si>
   <si>
-    <t>status.closed_marked_for_deletion</t>
-  </si>
-  <si>
     <t>closed-marked-for-deletion-claimed</t>
   </si>
   <si>
@@ -290,12 +224,108 @@
   </si>
   <si>
     <t>statusDescription.closed_marked_for_deletion</t>
+  </si>
+  <si>
+    <t>substatus</t>
+  </si>
+  <si>
+    <t>open_partially-completed</t>
+  </si>
+  <si>
+    <t>open_needs-follow-up</t>
+  </si>
+  <si>
+    <t>closed_out-of-scope</t>
+  </si>
+  <si>
+    <t>closed_done-by-others</t>
+  </si>
+  <si>
+    <t>closed_no-help-wanted</t>
+  </si>
+  <si>
+    <t>closed_marked-for-deletion</t>
+  </si>
+  <si>
+    <t>closed_partially-completed</t>
+  </si>
+  <si>
+    <t>status_name_t</t>
+  </si>
+  <si>
+    <t>substatus_name_t</t>
+  </si>
+  <si>
+    <t>description_t</t>
+  </si>
+  <si>
+    <t>claimed_class</t>
+  </si>
+  <si>
+    <t>unclaimed_class</t>
+  </si>
+  <si>
+    <t>completed_by_anybody</t>
+  </si>
+  <si>
+    <t>completed_by_ccu</t>
+  </si>
+  <si>
+    <t>completed_db</t>
+  </si>
+  <si>
+    <t>last_updated</t>
+  </si>
+  <si>
+    <t>depreciated_date</t>
+  </si>
+  <si>
+    <t>unassigned</t>
+  </si>
+  <si>
+    <t>assigned</t>
+  </si>
+  <si>
+    <t>partially-completed</t>
+  </si>
+  <si>
+    <t>needs-follow-up</t>
+  </si>
+  <si>
+    <t>unresponsive</t>
+  </si>
+  <si>
+    <t>completed</t>
+  </si>
+  <si>
+    <t>incomplete</t>
+  </si>
+  <si>
+    <t>out-of-scope</t>
+  </si>
+  <si>
+    <t>done-by-others</t>
+  </si>
+  <si>
+    <t>no-help-wanted</t>
+  </si>
+  <si>
+    <t>rejected</t>
+  </si>
+  <si>
+    <t>duplicate</t>
+  </si>
+  <si>
+    <t>marked-for-deletion</t>
+  </si>
+  <si>
+    <t>primary_state, status, substatus, status_name_t, substatus_name_t, description_t, claimed_class, unclaimed_class, completed_by_anybody, completed_by_ccu, completed_db, last_updated, depreciated_date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1130,19 +1160,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18:E28"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1150,947 +1184,1060 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L1" t="s">
+        <v>84</v>
+      </c>
+      <c r="M1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" t="str">
+        <f>"status."&amp;B2</f>
+        <v>status.open_unassigned</v>
+      </c>
+      <c r="E2" t="str">
+        <f>"substatus."&amp;C2</f>
+        <v>substatus.unassigned</v>
+      </c>
+      <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H2" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
         <v>43137</v>
       </c>
-      <c r="K2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" t="str">
-        <f>"  ('"&amp;A2&amp;"', '"&amp;B2&amp;"', '"&amp;C2&amp;"', '"&amp;D2&amp;"', '"&amp;E2&amp;"', '"&amp;F2&amp;"', "&amp;TEXT(G2,"0.00")&amp;", "&amp;TEXT(H2,"0.00")&amp;", "&amp;TEXT(I2,"0.00")&amp;", '"&amp;TEXT(J2,"YYYY-MM-DD")&amp;"', NULL),"</f>
-        <v xml:space="preserve">  ('open', 'open_unassigned', 'status.open_unassigned', 'statusDescription.open_unassigned', 'open-unassigned-claimed', 'open-unassigned-unclaimed', 0.00, 0.00, 0.00, '2018-02-06', NULL),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" t="str">
+        <f>"  ('"&amp;A2&amp;"', '"&amp;B2&amp;"', '"&amp;C2&amp;"', '"&amp;D2&amp;"', '"&amp;E2&amp;"', '"&amp;F2&amp;"', '"&amp;G2&amp;"', '"&amp;H2&amp;"', "&amp;TEXT(I2,"0.00")&amp;", "&amp;TEXT(J2,"0.00")&amp;", "&amp;TEXT(K2,"0.00")&amp;", '"&amp;TEXT(L2,"YYYY-MM-DD")&amp;"', "&amp;IF(M2="null","null","'"&amp;TEXT(M2,"YYYY-MM-DD")&amp;"'")&amp;"),"</f>
+        <v xml:space="preserve">  ('open', 'open_unassigned', 'unassigned', 'status.open_unassigned', 'substatus.unassigned', 'statusDescription.open_unassigned', 'open-unassigned-claimed', 'open-unassigned-unclaimed', 0.00, 0.00, 0.00, '2018-02-06', null),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
+        <v>87</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D14" si="0">"status."&amp;B3</f>
+        <v>status.open_assigned</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E14" si="1">"substatus."&amp;C3</f>
+        <v>substatus.assigned</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3">
-        <v>0.25</v>
-      </c>
-      <c r="H3">
-        <v>0.25</v>
+        <v>56</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
       </c>
       <c r="I3">
         <v>0.25</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3">
+        <v>0.25</v>
+      </c>
+      <c r="K3">
+        <v>0.25</v>
+      </c>
+      <c r="L3" s="1">
         <v>43137</v>
       </c>
-      <c r="K3" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" t="str">
-        <f t="shared" ref="M3:M14" si="0">"  ('"&amp;A3&amp;"', '"&amp;B3&amp;"', '"&amp;C3&amp;"', '"&amp;D3&amp;"', '"&amp;E3&amp;"', '"&amp;F3&amp;"', "&amp;TEXT(G3,"0.00")&amp;", "&amp;TEXT(H3,"0.00")&amp;", "&amp;TEXT(I3,"0.00")&amp;", '"&amp;TEXT(J3,"YYYY-MM-DD")&amp;"', NULL),"</f>
-        <v xml:space="preserve">  ('open', 'open_assigned', 'status.open_assigned', 'statusDescription.open_assigned', 'open-assigned-claimed', 'open-assigned-unclaimed', 0.25, 0.25, 0.25, '2018-02-06', NULL),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" t="str">
+        <f t="shared" ref="O3:O14" si="2">"  ('"&amp;A3&amp;"', '"&amp;B3&amp;"', '"&amp;C3&amp;"', '"&amp;D3&amp;"', '"&amp;E3&amp;"', '"&amp;F3&amp;"', '"&amp;G3&amp;"', '"&amp;H3&amp;"', "&amp;TEXT(I3,"0.00")&amp;", "&amp;TEXT(J3,"0.00")&amp;", "&amp;TEXT(K3,"0.00")&amp;", '"&amp;TEXT(L3,"YYYY-MM-DD")&amp;"', "&amp;IF(M3="null","null","'"&amp;TEXT(M3,"YYYY-MM-DD")&amp;"'")&amp;"),"</f>
+        <v xml:space="preserve">  ('open', 'open_assigned', 'assigned', 'status.open_assigned', 'substatus.assigned', 'statusDescription.open_assigned', 'open-assigned-claimed', 'open-assigned-unclaimed', 0.25, 0.25, 0.25, '2018-02-06', null),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>status.open_partially-completed</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="1"/>
+        <v>substatus.partially-completed</v>
+      </c>
+      <c r="F4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4">
-        <v>0.5</v>
-      </c>
-      <c r="H4">
-        <v>0.5</v>
+      <c r="H4" t="s">
+        <v>12</v>
       </c>
       <c r="I4">
         <v>0.5</v>
       </c>
-      <c r="J4" s="1">
-        <v>43137</v>
-      </c>
-      <c r="K4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M4" t="str">
+      <c r="J4">
+        <v>0.5</v>
+      </c>
+      <c r="K4">
+        <v>0.5</v>
+      </c>
+      <c r="L4" s="1">
+        <v>43441</v>
+      </c>
+      <c r="M4" t="s">
+        <v>6</v>
+      </c>
+      <c r="O4" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  ('open', 'open_partially-completed', 'partially-completed', 'status.open_partially-completed', 'substatus.partially-completed', 'statusDescription.open_partially_completed', 'open-partially-completed-claimed', 'open-partially-completed-unclaimed', 0.50, 0.50, 0.50, '2018-12-07', null),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  ('open', 'open_partially_completed', 'status.open_partially_completed', 'statusDescription.open_partially_completed', 'open-partially-completed-claimed', 'open-partially-completed-unclaimed', 0.50, 0.50, 0.50, '2018-02-06', NULL),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
+        <v>status.open_needs-follow-up</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="1"/>
+        <v>substatus.needs-follow-up</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5">
-        <v>0.5</v>
-      </c>
-      <c r="H5">
-        <v>0.5</v>
+        <v>58</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
       </c>
       <c r="I5">
         <v>0.5</v>
       </c>
-      <c r="J5" s="1">
-        <v>43137</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="J5">
+        <v>0.5</v>
+      </c>
+      <c r="K5">
+        <v>0.5</v>
+      </c>
+      <c r="L5" s="1">
+        <v>43441</v>
+      </c>
+      <c r="M5" t="s">
+        <v>6</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  ('open', 'open_needs-follow-up', 'needs-follow-up', 'status.open_needs-follow-up', 'substatus.needs-follow-up', 'statusDescription.open_needs_follow_up', 'open-needs-follow-up-claimed', 'open-needs-follow-up-unclaimed', 0.50, 0.50, 0.50, '2018-12-07', null),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="M5" t="str">
+      <c r="C6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  ('open', 'open_needs_follow_up', 'status.open_needs_follow_up', 'statusDescription.open_needs_follow_up', 'open-needs-follow-up-claimed', 'open-needs-follow-up-unclaimed', 0.50, 0.50, 0.50, '2018-02-06', NULL),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
+        <v>status.open_unresponsive</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>substatus.unresponsive</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6">
-        <v>0.1</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
+        <v>59</v>
+      </c>
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
       </c>
       <c r="I6">
         <v>0.1</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0.1</v>
+      </c>
+      <c r="L6" s="1">
         <v>43137</v>
       </c>
-      <c r="K6" t="s">
-        <v>16</v>
-      </c>
-      <c r="M6" t="str">
+      <c r="M6" t="s">
+        <v>6</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  ('open', 'open_unresponsive', 'unresponsive', 'status.open_unresponsive', 'substatus.unresponsive', 'statusDescription.open_unresponsive', 'open-unresponsive-claimed', 'open-unresponsive-unclaimed', 0.10, 0.00, 0.10, '2018-02-06', null),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  ('open', 'open_unresponsive', 'status.open_unresponsive', 'statusDescription.open_unresponsive', 'open-unresponsive-claimed', 'open-unresponsive-unclaimed', 0.10, 0.00, 0.10, '2018-02-06', NULL),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" t="s">
-        <v>36</v>
+        <v>status.closed_partially-completed</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>substatus.completed</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
+        <v>60</v>
+      </c>
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" t="s">
+        <v>22</v>
       </c>
       <c r="I7">
         <v>1</v>
       </c>
-      <c r="J7" s="1">
-        <v>43137</v>
-      </c>
-      <c r="K7" t="s">
-        <v>16</v>
-      </c>
-      <c r="M7" t="str">
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1">
+        <v>43441</v>
+      </c>
+      <c r="M7" t="s">
+        <v>6</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  ('closed', 'closed_partially-completed', 'completed', 'status.closed_partially-completed', 'substatus.completed', 'statusDescription.closed_completed', 'closed-completed-claimed', 'closed-completed-unclaimed', 1.00, 1.00, 1.00, '2018-12-07', null),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  ('closed', 'closed_completed', 'status.closed_completed', 'statusDescription.closed_completed', 'closed-completed-claimed', 'closed-completed-unclaimed', 1.00, 1.00, 1.00, '2018-02-06', NULL),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" t="s">
-        <v>83</v>
-      </c>
-      <c r="E8" t="s">
-        <v>40</v>
+        <v>status.closed_incomplete</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>substatus.incomplete</v>
       </c>
       <c r="F8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8">
-        <v>0.75</v>
-      </c>
-      <c r="H8">
-        <v>0.75</v>
+        <v>61</v>
+      </c>
+      <c r="G8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" t="s">
+        <v>25</v>
       </c>
       <c r="I8">
         <v>0.75</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8">
+        <v>0.75</v>
+      </c>
+      <c r="K8">
+        <v>0.75</v>
+      </c>
+      <c r="L8" s="1">
         <v>43137</v>
       </c>
-      <c r="K8" t="s">
-        <v>16</v>
-      </c>
-      <c r="M8" t="str">
+      <c r="M8" t="s">
+        <v>6</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  ('closed', 'closed_incomplete', 'incomplete', 'status.closed_incomplete', 'substatus.incomplete', 'statusDescription.closed_incomplete', 'closed-incomplete-claimed', 'closed-incomplete-unclaimed', 0.75, 0.75, 0.75, '2018-02-06', null),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  ('closed', 'closed_incomplete', 'status.closed_incomplete', 'statusDescription.closed_incomplete', 'closed-incomplete-claimed', 'closed-incomplete-unclaimed', 0.75, 0.75, 0.75, '2018-02-06', NULL),</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9" t="s">
-        <v>44</v>
+        <v>status.closed_out-of-scope</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>substatus.out-of-scope</v>
       </c>
       <c r="F9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9">
-        <v>0.25</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
+        <v>62</v>
+      </c>
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" t="s">
+        <v>28</v>
       </c>
       <c r="I9">
         <v>0.25</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0.25</v>
+      </c>
+      <c r="L9" s="1">
         <v>43137</v>
       </c>
-      <c r="K9" t="s">
-        <v>16</v>
-      </c>
-      <c r="M9" t="str">
+      <c r="M9" t="s">
+        <v>6</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  ('closed', 'closed_out-of-scope', 'out-of-scope', 'status.closed_out-of-scope', 'substatus.out-of-scope', 'statusDescription.closed_out_of_scope', 'closed-out-of-scope-claimed', 'closed-out-of-scope-unclaimed', 0.25, 0.00, 0.25, '2018-02-06', null),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  ('closed', 'closed_out_of_scope', 'status.closed_out_of_scope', 'statusDescription.closed_out_of_scope', 'closed-out-of-scope-claimed', 'closed-out-of-scope-unclaimed', 0.25, 0.00, 0.25, '2018-02-06', NULL),</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" t="s">
-        <v>85</v>
-      </c>
-      <c r="E10" t="s">
-        <v>48</v>
+        <v>status.closed_done-by-others</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>substatus.done-by-others</v>
       </c>
       <c r="F10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
+        <v>63</v>
+      </c>
+      <c r="G10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" t="s">
+        <v>31</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
-      <c r="J10" s="1">
-        <v>43137</v>
-      </c>
-      <c r="K10" t="s">
-        <v>16</v>
-      </c>
-      <c r="M10" t="str">
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10" s="1">
+        <v>43441</v>
+      </c>
+      <c r="M10" t="s">
+        <v>6</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  ('closed', 'closed_done-by-others', 'done-by-others', 'status.closed_done-by-others', 'substatus.done-by-others', 'statusDescription.closed_done_by_others', 'closed-done-by-others-claimed', 'closed-done-by-others-unclaimed', 1.00, 0.00, 1.00, '2018-12-07', null),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  ('closed', 'closed_done_by_others', 'status.closed_done_by_others', 'statusDescription.closed_done_by_others', 'closed-done-by-others-claimed', 'closed-done-by-others-unclaimed', 1.00, 0.00, 1.00, '2018-02-06', NULL),</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+        <v>status.closed_no-help-wanted</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>substatus.no-help-wanted</v>
+      </c>
+      <c r="F11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" t="s">
         <v>33</v>
       </c>
-      <c r="B11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E11" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
+      <c r="H11" t="s">
+        <v>34</v>
       </c>
       <c r="I11">
         <v>1</v>
       </c>
-      <c r="J11" s="1">
-        <v>43137</v>
-      </c>
-      <c r="K11" t="s">
-        <v>16</v>
-      </c>
-      <c r="M11" t="str">
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1">
+        <v>43441</v>
+      </c>
+      <c r="M11" t="s">
+        <v>6</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  ('closed', 'closed_no-help-wanted', 'no-help-wanted', 'status.closed_no-help-wanted', 'substatus.no-help-wanted', 'statusDescription.closed_no_help_wanted', 'closed-no-help-wanted-claimed', 'closed-no-help-wanted-unclaimed', 1.00, 0.00, 1.00, '2018-12-07', null),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  ('closed', 'closed_no_help_wanted', 'status.closed_no_help_wanted', 'statusDescription.closed_no_help_wanted', 'closed-no-help-wanted-claimed', 'closed-no-help-wanted-unclaimed', 1.00, 0.00, 1.00, '2018-02-06', NULL),</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" t="s">
-        <v>87</v>
-      </c>
-      <c r="E12" t="s">
-        <v>56</v>
+        <v>status.closed_rejected</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>substatus.rejected</v>
       </c>
       <c r="F12" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12">
-        <v>0.25</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
+        <v>65</v>
+      </c>
+      <c r="G12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" t="s">
+        <v>37</v>
       </c>
       <c r="I12">
         <v>0.25</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0.25</v>
+      </c>
+      <c r="L12" s="1">
         <v>43137</v>
       </c>
-      <c r="K12" t="s">
-        <v>16</v>
-      </c>
-      <c r="M12" t="str">
+      <c r="M12" t="s">
+        <v>6</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  ('closed', 'closed_rejected', 'rejected', 'status.closed_rejected', 'substatus.rejected', 'statusDescription.closed_rejected', 'closed-rejected-claimed', 'closed-rejected-unclaimed', 0.25, 0.00, 0.25, '2018-02-06', null),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  ('closed', 'closed_rejected', 'status.closed_rejected', 'statusDescription.closed_rejected', 'closed-rejected-claimed', 'closed-rejected-unclaimed', 0.25, 0.00, 0.25, '2018-02-06', NULL),</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" t="s">
-        <v>88</v>
-      </c>
-      <c r="E13" t="s">
-        <v>60</v>
+        <v>status.closed_duplicate</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>substatus.duplicate</v>
       </c>
       <c r="F13" t="s">
-        <v>61</v>
-      </c>
-      <c r="G13">
+        <v>66</v>
+      </c>
+      <c r="G13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13">
         <v>0</v>
       </c>
-      <c r="H13">
+      <c r="J13">
         <v>0</v>
       </c>
-      <c r="I13">
+      <c r="K13">
         <v>1</v>
       </c>
-      <c r="J13" s="1">
+      <c r="L13" s="1">
         <v>43137</v>
       </c>
-      <c r="K13" t="s">
-        <v>16</v>
-      </c>
-      <c r="M13" t="str">
+      <c r="M13" t="s">
+        <v>6</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  ('closed', 'closed_duplicate', 'duplicate', 'status.closed_duplicate', 'substatus.duplicate', 'statusDescription.closed_duplicate', 'closed-duplicate-claimed', 'closed-duplicate-unclaimed', 0.00, 0.00, 1.00, '2018-02-06', null),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">  ('closed', 'closed_duplicate', 'status.closed_duplicate', 'statusDescription.closed_duplicate', 'closed-duplicate-claimed', 'closed-duplicate-unclaimed', 0.00, 0.00, 1.00, '2018-02-06', NULL),</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" t="s">
-        <v>89</v>
-      </c>
-      <c r="E14" t="s">
-        <v>64</v>
+        <v>status.closed_marked-for-deletion</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>substatus.marked-for-deletion</v>
       </c>
       <c r="F14" t="s">
-        <v>65</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
+        <v>67</v>
+      </c>
+      <c r="G14" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14" t="s">
+        <v>43</v>
       </c>
       <c r="I14">
         <v>0</v>
       </c>
-      <c r="J14" s="1">
-        <v>43137</v>
-      </c>
-      <c r="K14" t="s">
-        <v>16</v>
-      </c>
-      <c r="M14" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">  ('closed', 'closed_marked_for_deletion', 'status.closed_marked_for_deletion', 'statusDescription.closed_marked_for_deletion', 'closed-marked-for-deletion-claimed', 'closed-marked-for-deletion-unclaimed', 0.00, 0.00, 0.00, '2018-02-06', NULL),</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
+        <v>43441</v>
+      </c>
+      <c r="M14" t="s">
+        <v>6</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">  ('closed', 'closed_marked-for-deletion', 'marked-for-deletion', 'status.closed_marked-for-deletion', 'substatus.marked-for-deletion', 'statusDescription.closed_marked_for_deletion', 'closed-marked-for-deletion-claimed', 'closed-marked-for-deletion-unclaimed', 0.00, 0.00, 0.00, '2018-12-07', null),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" t="str">
+        <v>44</v>
+      </c>
+      <c r="D18" t="str">
         <f>VLOOKUP(A18,$A$30:$B$42,2,FALSE)</f>
         <v>open_unassigned</v>
       </c>
-      <c r="E18" t="str">
-        <f>"UPDATE public.core_worksites SET status_key = '"&amp;C18&amp;"' WHERE status = '"&amp;B18&amp;"';"</f>
+      <c r="G18" t="str">
+        <f>"UPDATE public.core_worksites SET status_key = '"&amp;D18&amp;"' WHERE status = '"&amp;B18&amp;"';"</f>
         <v>UPDATE public.core_worksites SET status_key = 'open_unassigned' WHERE status = 'Open, unassigned';</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" t="str">
-        <f t="shared" ref="C19:C28" si="1">VLOOKUP(A19,$A$30:$B$42,2,FALSE)</f>
+        <v>51</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" ref="D19:D28" si="3">VLOOKUP(A19,$A$30:$B$42,2,FALSE)</f>
         <v>open_partially_completed</v>
       </c>
-      <c r="E19" t="str">
-        <f t="shared" ref="E19:E28" si="2">"UPDATE public.core_worksites SET status_key = '"&amp;C19&amp;"' WHERE status = '"&amp;B19&amp;"';"</f>
+      <c r="G19" t="str">
+        <f>"UPDATE public.core_worksites SET status_key = '"&amp;D19&amp;"' WHERE status = '"&amp;B19&amp;"';"</f>
         <v>UPDATE public.core_worksites SET status_key = 'open_partially_completed' WHERE status = 'Open, partially completed';</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" t="str">
-        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="3"/>
         <v>open_needs_follow_up</v>
       </c>
-      <c r="E20" t="str">
-        <f t="shared" si="2"/>
+      <c r="G20" t="str">
+        <f>"UPDATE public.core_worksites SET status_key = '"&amp;D20&amp;"' WHERE status = '"&amp;B20&amp;"';"</f>
         <v>UPDATE public.core_worksites SET status_key = 'open_needs_follow_up' WHERE status = 'Open, needs follow-up';</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" t="str">
-        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="3"/>
         <v>open_assigned</v>
       </c>
-      <c r="E21" t="str">
-        <f t="shared" si="2"/>
+      <c r="G21" t="str">
+        <f>"UPDATE public.core_worksites SET status_key = '"&amp;D21&amp;"' WHERE status = '"&amp;B21&amp;"';"</f>
         <v>UPDATE public.core_worksites SET status_key = 'open_assigned' WHERE status = 'Open, assigned';</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" t="str">
-        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="3"/>
         <v>closed_rejected</v>
       </c>
-      <c r="E22" t="str">
-        <f t="shared" si="2"/>
+      <c r="G22" t="str">
+        <f>"UPDATE public.core_worksites SET status_key = '"&amp;D22&amp;"' WHERE status = '"&amp;B22&amp;"';"</f>
         <v>UPDATE public.core_worksites SET status_key = 'closed_rejected' WHERE status = 'Closed, rejected';</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>76</v>
-      </c>
-      <c r="C23" t="str">
-        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="3"/>
         <v>closed_out_of_scope</v>
       </c>
-      <c r="E23" t="str">
-        <f t="shared" si="2"/>
+      <c r="G23" t="str">
+        <f>"UPDATE public.core_worksites SET status_key = '"&amp;D23&amp;"' WHERE status = '"&amp;B23&amp;"';"</f>
         <v>UPDATE public.core_worksites SET status_key = 'closed_out_of_scope' WHERE status = 'Closed, out of scope';</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
-      </c>
-      <c r="C24" t="str">
-        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="3"/>
         <v>closed_no_help_wanted</v>
       </c>
-      <c r="E24" t="str">
-        <f t="shared" si="2"/>
+      <c r="G24" t="str">
+        <f>"UPDATE public.core_worksites SET status_key = '"&amp;D24&amp;"' WHERE status = '"&amp;B24&amp;"';"</f>
         <v>UPDATE public.core_worksites SET status_key = 'closed_no_help_wanted' WHERE status = 'Closed, no help wanted';</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>68</v>
-      </c>
-      <c r="C25" t="str">
-        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="3"/>
         <v>closed_incomplete</v>
       </c>
-      <c r="E25" t="str">
-        <f t="shared" si="2"/>
+      <c r="G25" t="str">
+        <f>"UPDATE public.core_worksites SET status_key = '"&amp;D25&amp;"' WHERE status = '"&amp;B25&amp;"';"</f>
         <v>UPDATE public.core_worksites SET status_key = 'closed_incomplete' WHERE status = 'Closed, incomplete';</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" t="str">
-        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="3"/>
         <v>closed_duplicate</v>
       </c>
-      <c r="E26" t="str">
-        <f t="shared" si="2"/>
+      <c r="G26" t="str">
+        <f>"UPDATE public.core_worksites SET status_key = '"&amp;D26&amp;"' WHERE status = '"&amp;B26&amp;"';"</f>
         <v>UPDATE public.core_worksites SET status_key = 'closed_duplicate' WHERE status = 'Closed, duplicate';</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" t="str">
-        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="3"/>
         <v>closed_done_by_others</v>
       </c>
-      <c r="E27" t="str">
-        <f t="shared" si="2"/>
+      <c r="G27" t="str">
+        <f>"UPDATE public.core_worksites SET status_key = '"&amp;D27&amp;"' WHERE status = '"&amp;B27&amp;"';"</f>
         <v>UPDATE public.core_worksites SET status_key = 'closed_done_by_others' WHERE status = 'Closed, done by others';</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>72</v>
-      </c>
-      <c r="C28" t="str">
-        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="3"/>
         <v>closed_completed</v>
       </c>
-      <c r="E28" t="str">
-        <f t="shared" si="2"/>
+      <c r="G28" t="str">
+        <f>"UPDATE public.core_worksites SET status_key = '"&amp;D28&amp;"' WHERE status = '"&amp;B28&amp;"';"</f>
         <v>UPDATE public.core_worksites SET status_key = 'closed_completed' WHERE status = 'Closed, completed';</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30">
+        <v>3</v>
+      </c>
+      <c r="D30">
         <v>1</v>
       </c>
-      <c r="D30" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" t="str">
-        <f>IF(AND(A30=C30,B30=D30),"","problem")</f>
+      <c r="F30" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" t="str">
+        <f>IF(AND(A30=D30,B30=F30),"","problem")</f>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31">
+        <v>7</v>
+      </c>
+      <c r="D31">
         <v>2</v>
       </c>
-      <c r="D31" t="s">
-        <v>17</v>
-      </c>
-      <c r="E31" t="str">
-        <f t="shared" ref="E31:E42" si="3">IF(AND(A31=C31,B31=D31),"","problem")</f>
+      <c r="F31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" t="str">
+        <f>IF(AND(A31=D31,B31=F31),"","problem")</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C32">
+        <v>10</v>
+      </c>
+      <c r="D32">
         <v>3</v>
       </c>
-      <c r="D32" t="s">
-        <v>21</v>
-      </c>
-      <c r="E32" t="str">
-        <f t="shared" si="3"/>
+      <c r="F32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" t="str">
+        <f>IF(AND(A32=D32,B32=F32),"","problem")</f>
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33">
+        <v>13</v>
+      </c>
+      <c r="D33">
         <v>4</v>
       </c>
-      <c r="D33" t="s">
-        <v>25</v>
-      </c>
-      <c r="E33" t="str">
-        <f t="shared" si="3"/>
+      <c r="F33" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" t="str">
+        <f>IF(AND(A33=D33,B33=F33),"","problem")</f>
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34">
+        <v>16</v>
+      </c>
+      <c r="D34">
         <v>5</v>
       </c>
-      <c r="D34" t="s">
-        <v>29</v>
-      </c>
-      <c r="E34" t="str">
-        <f t="shared" si="3"/>
+      <c r="F34" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" t="str">
+        <f>IF(AND(A34=D34,B34=F34),"","problem")</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>6</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35">
+        <v>20</v>
+      </c>
+      <c r="D35">
         <v>6</v>
       </c>
-      <c r="D35" t="s">
-        <v>34</v>
-      </c>
-      <c r="E35" t="str">
-        <f t="shared" si="3"/>
+      <c r="F35" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" t="str">
+        <f>IF(AND(A35=D35,B35=F35),"","problem")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
-      </c>
-      <c r="C36">
+        <v>23</v>
+      </c>
+      <c r="D36">
         <v>7</v>
       </c>
-      <c r="D36" t="s">
-        <v>38</v>
-      </c>
-      <c r="E36" t="str">
-        <f t="shared" si="3"/>
+      <c r="F36" t="s">
+        <v>23</v>
+      </c>
+      <c r="G36" t="str">
+        <f>IF(AND(A36=D36,B36=F36),"","problem")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
-      </c>
-      <c r="C37">
+        <v>26</v>
+      </c>
+      <c r="D37">
         <v>8</v>
       </c>
-      <c r="D37" t="s">
-        <v>42</v>
-      </c>
-      <c r="E37" t="str">
-        <f t="shared" si="3"/>
+      <c r="F37" t="s">
+        <v>26</v>
+      </c>
+      <c r="G37" t="str">
+        <f>IF(AND(A37=D37,B37=F37),"","problem")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38">
+        <v>29</v>
+      </c>
+      <c r="D38">
         <v>9</v>
       </c>
-      <c r="D38" t="s">
-        <v>46</v>
-      </c>
-      <c r="E38" t="str">
-        <f t="shared" si="3"/>
+      <c r="F38" t="s">
+        <v>29</v>
+      </c>
+      <c r="G38" t="str">
+        <f>IF(AND(A38=D38,B38=F38),"","problem")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>50</v>
-      </c>
-      <c r="C39">
+        <v>32</v>
+      </c>
+      <c r="D39">
         <v>10</v>
       </c>
-      <c r="D39" t="s">
-        <v>50</v>
-      </c>
-      <c r="E39" t="str">
-        <f t="shared" si="3"/>
+      <c r="F39" t="s">
+        <v>32</v>
+      </c>
+      <c r="G39" t="str">
+        <f>IF(AND(A39=D39,B39=F39),"","problem")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>54</v>
-      </c>
-      <c r="C40">
+        <v>35</v>
+      </c>
+      <c r="D40">
         <v>11</v>
       </c>
-      <c r="D40" t="s">
-        <v>54</v>
-      </c>
-      <c r="E40" t="str">
-        <f t="shared" si="3"/>
+      <c r="F40" t="s">
+        <v>35</v>
+      </c>
+      <c r="G40" t="str">
+        <f>IF(AND(A40=D40,B40=F40),"","problem")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>58</v>
-      </c>
-      <c r="C41">
+        <v>38</v>
+      </c>
+      <c r="D41">
         <v>12</v>
       </c>
-      <c r="D41" t="s">
-        <v>58</v>
-      </c>
-      <c r="E41" t="str">
-        <f t="shared" si="3"/>
+      <c r="F41" t="s">
+        <v>38</v>
+      </c>
+      <c r="G41" t="str">
+        <f>IF(AND(A41=D41,B41=F41),"","problem")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>62</v>
-      </c>
-      <c r="C42">
+        <v>41</v>
+      </c>
+      <c r="D42">
         <v>13</v>
       </c>
-      <c r="D42" t="s">
-        <v>62</v>
-      </c>
-      <c r="E42" t="str">
-        <f t="shared" si="3"/>
+      <c r="F42" t="s">
+        <v>41</v>
+      </c>
+      <c r="G42" t="str">
+        <f>IF(AND(A42=D42,B42=F42),"","problem")</f>
         <v/>
       </c>
     </row>
@@ -2099,5 +2246,6 @@
     <sortCondition descending="1" ref="B18:B28"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>